<commit_message>
Core done for one fabricator
Now moving on to Tkinter for the use friendly interface
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -538,12 +538,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t xml:space="preserve">360.00 </t>
+          <t>360.00</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>MCP1754ST-5002E/DB</t>
+          <t xml:space="preserve"> MCP1754ST-5002E/DB</t>
         </is>
       </c>
     </row>
@@ -595,12 +595,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>3k3</t>
+          <t xml:space="preserve"> 3k3</t>
         </is>
       </c>
     </row>
@@ -652,12 +652,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -709,12 +709,12 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -766,12 +766,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t xml:space="preserve">180.00 </t>
+          <t>180.00</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>691 253 510 002 &amp; 003</t>
+          <t xml:space="preserve"> 691 253 510 002 &amp; 003</t>
         </is>
       </c>
     </row>
@@ -823,12 +823,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>FINDER-4032</t>
+          <t xml:space="preserve"> FINDER-4032</t>
         </is>
       </c>
     </row>
@@ -880,12 +880,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>PIC PROGRAM</t>
+          <t xml:space="preserve"> PIC PROGRAM</t>
         </is>
       </c>
     </row>
@@ -937,12 +937,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>PIC PROGRAM</t>
+          <t xml:space="preserve"> PIC PROGRAM</t>
         </is>
       </c>
     </row>
@@ -994,12 +994,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BC847</t>
+          <t xml:space="preserve"> BC847</t>
         </is>
       </c>
     </row>
@@ -1051,12 +1051,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1108,12 +1108,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1165,12 +1165,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1222,12 +1222,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1279,12 +1279,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1336,12 +1336,12 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BC847</t>
+          <t xml:space="preserve"> BC847</t>
         </is>
       </c>
     </row>
@@ -1393,12 +1393,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1450,12 +1450,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1507,12 +1507,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1564,12 +1564,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -1621,12 +1621,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>1k5</t>
+          <t xml:space="preserve"> 1k5</t>
         </is>
       </c>
     </row>
@@ -1678,12 +1678,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -1735,12 +1735,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>47k</t>
+          <t xml:space="preserve"> 47k</t>
         </is>
       </c>
     </row>
@@ -1792,12 +1792,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>12k</t>
+          <t xml:space="preserve"> 12k</t>
         </is>
       </c>
     </row>
@@ -1849,12 +1849,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t xml:space="preserve">180.00 </t>
+          <t>180.00</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -1906,12 +1906,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2k</t>
+          <t xml:space="preserve"> 2k</t>
         </is>
       </c>
     </row>
@@ -1963,12 +1963,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>680E</t>
+          <t xml:space="preserve"> 680E</t>
         </is>
       </c>
     </row>
@@ -2020,12 +2020,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>470E</t>
+          <t xml:space="preserve"> 470E</t>
         </is>
       </c>
     </row>
@@ -2077,12 +2077,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>220E</t>
+          <t xml:space="preserve"> 220E</t>
         </is>
       </c>
     </row>
@@ -2134,12 +2134,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -2191,12 +2191,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -2248,12 +2248,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -2305,12 +2305,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -2362,12 +2362,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>1k5</t>
+          <t xml:space="preserve"> 1k5</t>
         </is>
       </c>
     </row>
@@ -2419,12 +2419,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -2476,12 +2476,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>47k</t>
+          <t xml:space="preserve"> 47k</t>
         </is>
       </c>
     </row>
@@ -2533,12 +2533,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>12k</t>
+          <t xml:space="preserve"> 12k</t>
         </is>
       </c>
     </row>
@@ -2590,12 +2590,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">180.00 </t>
+          <t>180.00</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -2647,12 +2647,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>910E</t>
+          <t xml:space="preserve"> 910E</t>
         </is>
       </c>
     </row>
@@ -2704,12 +2704,12 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>750E</t>
+          <t xml:space="preserve"> 750E</t>
         </is>
       </c>
     </row>
@@ -2761,12 +2761,12 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>620E</t>
+          <t xml:space="preserve"> 620E</t>
         </is>
       </c>
     </row>
@@ -2818,12 +2818,12 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>510E</t>
+          <t xml:space="preserve"> 510E</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2875,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t xml:space="preserve">360.00 </t>
+          <t>360.00</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>11k5</t>
+          <t xml:space="preserve"> 11k5</t>
         </is>
       </c>
     </row>
@@ -2932,12 +2932,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -2989,12 +2989,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -3046,12 +3046,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -3103,12 +3103,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>22k</t>
+          <t xml:space="preserve"> 22k</t>
         </is>
       </c>
     </row>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>LM358</t>
+          <t xml:space="preserve"> LM358</t>
         </is>
       </c>
     </row>
@@ -3217,12 +3217,12 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>PIC16F1826</t>
+          <t xml:space="preserve"> PIC16F1826</t>
         </is>
       </c>
     </row>
@@ -3274,12 +3274,12 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>LM358</t>
+          <t xml:space="preserve"> LM358</t>
         </is>
       </c>
     </row>
@@ -3331,12 +3331,12 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>PIC16F1826</t>
+          <t xml:space="preserve"> PIC16F1826</t>
         </is>
       </c>
     </row>
@@ -3388,12 +3388,12 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t xml:space="preserve">360.00 </t>
+          <t>360.00</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>BAV70</t>
+          <t xml:space="preserve"> BAV70</t>
         </is>
       </c>
     </row>
@@ -3445,12 +3445,12 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t xml:space="preserve">180.00 </t>
+          <t>180.00</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>ES1B</t>
+          <t xml:space="preserve"> ES1B</t>
         </is>
       </c>
     </row>
@@ -3502,12 +3502,12 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t xml:space="preserve">180.00 </t>
+          <t>180.00</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>ES1B</t>
+          <t xml:space="preserve"> ES1B</t>
         </is>
       </c>
     </row>
@@ -3559,12 +3559,12 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>10nF</t>
+          <t xml:space="preserve"> 10nF</t>
         </is>
       </c>
     </row>
@@ -3616,12 +3616,12 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t xml:space="preserve">180.00 </t>
+          <t>180.00</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>100n</t>
+          <t xml:space="preserve"> 100n</t>
         </is>
       </c>
     </row>
@@ -3673,12 +3673,12 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>100n</t>
+          <t xml:space="preserve"> 100n</t>
         </is>
       </c>
     </row>
@@ -3730,12 +3730,12 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>10nF</t>
+          <t xml:space="preserve"> 10nF</t>
         </is>
       </c>
     </row>
@@ -3787,12 +3787,12 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t xml:space="preserve">180.00 </t>
+          <t>180.00</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>100n</t>
+          <t xml:space="preserve"> 100n</t>
         </is>
       </c>
     </row>
@@ -3844,12 +3844,12 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>100n</t>
+          <t xml:space="preserve"> 100n</t>
         </is>
       </c>
     </row>
@@ -3901,12 +3901,12 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t xml:space="preserve">360.00 </t>
+          <t>360.00</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>ZEKERING</t>
+          <t xml:space="preserve"> ZEKERING</t>
         </is>
       </c>
     </row>
@@ -3958,12 +3958,12 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>VOM617A</t>
+          <t xml:space="preserve"> VOM617A</t>
         </is>
       </c>
     </row>
@@ -4015,12 +4015,12 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>ES1B</t>
+          <t xml:space="preserve"> ES1B</t>
         </is>
       </c>
     </row>
@@ -4072,12 +4072,12 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t xml:space="preserve">360.00 </t>
+          <t>360.00</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>691 243 310 008</t>
+          <t xml:space="preserve"> 691 243 310 008</t>
         </is>
       </c>
     </row>
@@ -4129,12 +4129,12 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>691 253 510 002</t>
+          <t xml:space="preserve"> 691 253 510 002</t>
         </is>
       </c>
     </row>
@@ -4186,12 +4186,12 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>691 253 510 003</t>
+          <t xml:space="preserve"> 691 253 510 003</t>
         </is>
       </c>
     </row>
@@ -4243,12 +4243,12 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t xml:space="preserve">360.00 </t>
+          <t>360.00</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t xml:space="preserve">PDTC114YT </t>
+          <t xml:space="preserve"> PDTC114YT </t>
         </is>
       </c>
     </row>
@@ -4300,12 +4300,12 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>220k</t>
+          <t xml:space="preserve"> 220k</t>
         </is>
       </c>
     </row>
@@ -4357,12 +4357,12 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>4k7</t>
+          <t xml:space="preserve"> 4k7</t>
         </is>
       </c>
     </row>
@@ -4414,12 +4414,12 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>ES1B</t>
+          <t xml:space="preserve"> ES1B</t>
         </is>
       </c>
     </row>
@@ -4471,12 +4471,12 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>10uF</t>
+          <t xml:space="preserve"> 10uF</t>
         </is>
       </c>
     </row>
@@ -4528,12 +4528,12 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>10uF</t>
+          <t xml:space="preserve"> 10uF</t>
         </is>
       </c>
     </row>
@@ -4585,12 +4585,12 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t xml:space="preserve">270.00 </t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>100n</t>
+          <t xml:space="preserve"> 100n</t>
         </is>
       </c>
     </row>
@@ -4642,12 +4642,12 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>REMOPA LOGO MIDDEL</t>
+          <t xml:space="preserve"> REMOPA LOGO MIDDEL</t>
         </is>
       </c>
     </row>
@@ -4699,12 +4699,12 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t xml:space="preserve">360.00 </t>
+          <t>360.00</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t xml:space="preserve">IRM-02-12 </t>
+          <t xml:space="preserve"> IRM-02-12 </t>
         </is>
       </c>
     </row>
@@ -4756,12 +4756,12 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t xml:space="preserve">90.00 </t>
+          <t>90.00</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>10uF</t>
+          <t xml:space="preserve"> 10uF</t>
         </is>
       </c>
     </row>
@@ -4813,12 +4813,12 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00 </t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>691 253 510 003</t>
+          <t xml:space="preserve"> 691 253 510 003</t>
         </is>
       </c>
     </row>

</xml_diff>